<commit_message>
update the structure so files don't throw errors when created
</commit_message>
<xml_diff>
--- a/create_data/Digital Skills Workshops 2021.xlsx
+++ b/create_data/Digital Skills Workshops 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nlesc.sharepoint.com/sites/instructors/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="295" documentId="6_{C80DD207-0A02-E949-8A39-41D0CCF88725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F54A2C45-1799-8F49-9CE9-7BE296CDD945}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="6_{C80DD207-0A02-E949-8A39-41D0CCF88725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06413E8F-D418-4DC1-9214-EB4D5490D256}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="178">
   <si>
     <t>Week of</t>
   </si>
@@ -580,13 +580,16 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>ds-docker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,7 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -724,8 +727,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -737,15 +738,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -761,6 +763,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -806,10 +811,10 @@
     <tableColumn id="13" xr3:uid="{70DDD074-33B8-49EA-AF94-6BA000F8013C}" name="helper1"/>
     <tableColumn id="14" xr3:uid="{BB43C387-FAFF-4DA0-928E-3C95D1CE2957}" name="helper2"/>
     <tableColumn id="15" xr3:uid="{EC9756CD-666D-44FA-9312-0F4D8701DD81}" name="helper3"/>
-    <tableColumn id="23" xr3:uid="{461ED2E0-A3DF-41CB-92E0-A4DCA3BC9ED6}" name="Comments" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{98451601-1ECB-4C6B-9478-91ABF4FB04D0}" name="starttime" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{B34968E8-53EF-40B6-A349-9E0BC6407F77}" name="endtime" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{7F8833F9-F100-2E4E-A711-C78FE6C566DE}" name="slug" dataDxfId="3">
+    <tableColumn id="23" xr3:uid="{461ED2E0-A3DF-41CB-92E0-A4DCA3BC9ED6}" name="Comments" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{98451601-1ECB-4C6B-9478-91ABF4FB04D0}" name="starttime" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B34968E8-53EF-40B6-A349-9E0BC6407F77}" name="endtime" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{7F8833F9-F100-2E4E-A711-C78FE6C566DE}" name="slug" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{0AD5F170-0BCD-457D-A8B2-FDB70BCB7E4E}" name="carpentry"/>
@@ -819,10 +824,10 @@
     <tableColumn id="20" xr3:uid="{A785A2E5-9541-4367-8FC5-939DEBB7BBC9}" name="venue"/>
     <tableColumn id="21" xr3:uid="{ABCA8351-9FE8-44D3-B755-D8323EB59496}" name="address"/>
     <tableColumn id="22" xr3:uid="{38057589-3894-4A27-851C-4CA96861394C}" name="country"/>
-    <tableColumn id="26" xr3:uid="{313E781C-A81E-A24B-BA89-66CDC0577AE5}" name="eventbrite" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{313E781C-A81E-A24B-BA89-66CDC0577AE5}" name="eventbrite" dataDxfId="1"/>
     <tableColumn id="1" xr3:uid="{FC1C6B11-AA2B-C048-8EE5-C5E41FB39B2D}" name="ready"/>
-    <tableColumn id="25" xr3:uid="{B66BA83E-B5CE-E34C-9152-38647FD62FF3}" name="repository" dataDxfId="1">
-      <calculatedColumnFormula>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</calculatedColumnFormula>
+    <tableColumn id="25" xr3:uid="{B66BA83E-B5CE-E34C-9152-38647FD62FF3}" name="repository" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{C61D59B8-B06F-491D-B188-9AAA39E41FEC}" name="oldslug"/>
   </tableColumns>
@@ -1139,43 +1144,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" customWidth="1"/>
-    <col min="7" max="7" width="23.5" customWidth="1"/>
-    <col min="8" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="19.83203125" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="28" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="28" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" customWidth="1"/>
-    <col min="23" max="23" width="18.5" customWidth="1"/>
-    <col min="24" max="24" width="11.83203125" customWidth="1"/>
-    <col min="25" max="25" width="20.6640625" style="18" customWidth="1"/>
-    <col min="26" max="26" width="12.83203125" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31.33203125" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" customWidth="1"/>
-    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5" style="23" customWidth="1"/>
-    <col min="36" max="36" width="62.33203125" customWidth="1"/>
-    <col min="37" max="37" width="165.5" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="26" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="26" customWidth="1"/>
+    <col min="15" max="15" width="32.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="25" max="25" width="53.85546875" style="18" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31.28515625" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="23" customWidth="1"/>
+    <col min="36" max="36" width="62.28515625" customWidth="1"/>
+    <col min="37" max="37" width="165.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1264,7 @@
       </c>
       <c r="AI1"/>
     </row>
-    <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:35" ht="18.75">
       <c r="A2" s="1">
         <v>44256</v>
       </c>
@@ -1276,12 +1284,12 @@
       </c>
       <c r="W2" s="23"/>
       <c r="Y2" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI2"/>
     </row>
-    <row r="3" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" s="2" customFormat="1">
       <c r="A3" s="3">
         <v>44263</v>
       </c>
@@ -1309,7 +1317,7 @@
       <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="L3" s="32" t="s">
         <v>41</v>
       </c>
       <c r="M3" s="24"/>
@@ -1330,6 +1338,9 @@
       <c r="S3" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1337,15 +1348,15 @@
       <c r="X3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y3" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-03-08-swc-gapminder-python-nlesc</v>
+      <c r="Y3" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-03-08-swc-gapminder-python-nlesc</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35">
       <c r="A4" s="1">
         <v>44270</v>
       </c>
@@ -1363,12 +1374,12 @@
       <c r="R4" s="2"/>
       <c r="W4" s="23"/>
       <c r="Y4" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI4"/>
     </row>
-    <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" s="2" customFormat="1">
       <c r="A5" s="3">
         <v>44277</v>
       </c>
@@ -1391,7 +1402,7 @@
       <c r="J5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="34"/>
+      <c r="L5" s="32"/>
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
       <c r="O5" s="4" t="str">
@@ -1404,6 +1415,9 @@
       <c r="Q5" t="s">
         <v>49</v>
       </c>
+      <c r="T5" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U5" s="2" t="s">
         <v>40</v>
       </c>
@@ -1411,15 +1425,15 @@
       <c r="X5" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y5" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-03-23-ds-containers</v>
+      <c r="Y5" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-03-23-ds-containers</v>
       </c>
       <c r="Z5" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" s="2" customFormat="1">
       <c r="A6" s="3">
         <v>44284</v>
       </c>
@@ -1444,7 +1458,7 @@
       <c r="J6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="34"/>
+      <c r="L6" s="32"/>
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
       <c r="O6" s="4" t="str">
@@ -1457,6 +1471,9 @@
       <c r="Q6" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="T6" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U6" s="2" t="s">
         <v>40</v>
       </c>
@@ -1464,15 +1481,15 @@
       <c r="X6" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y6" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-03-29-ds-cr</v>
+      <c r="Y6" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-03-29-ds-cr</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35">
       <c r="A7" s="1">
         <v>44291</v>
       </c>
@@ -1482,9 +1499,9 @@
       <c r="D7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
+      <c r="E7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
       <c r="O7" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
@@ -1492,12 +1509,12 @@
       <c r="R7" s="2"/>
       <c r="W7" s="23"/>
       <c r="Y7" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI7"/>
     </row>
-    <row r="8" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" s="2" customFormat="1">
       <c r="A8" s="3">
         <v>44298</v>
       </c>
@@ -1520,7 +1537,7 @@
       <c r="J8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="32" t="s">
         <v>64</v>
       </c>
       <c r="M8" s="24"/>
@@ -1535,6 +1552,9 @@
       <c r="Q8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="T8" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1542,15 +1562,15 @@
       <c r="X8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y8" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-04-12-ds-parallel</v>
+      <c r="Y8" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-04-12-ds-parallel</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" s="2" customFormat="1">
       <c r="A9" s="3">
         <v>44305</v>
       </c>
@@ -1576,7 +1596,7 @@
       <c r="K9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="L9" s="32" t="s">
         <v>72</v>
       </c>
       <c r="M9" s="24"/>
@@ -1597,6 +1617,9 @@
       <c r="S9" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="T9" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1604,15 +1627,15 @@
       <c r="X9" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y9" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-04-19-dc-ecology-python-nlesc</v>
+      <c r="Y9" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-04-19-dc-ecology-python-nlesc</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35">
       <c r="A10" s="1">
         <v>44312</v>
       </c>
@@ -1622,9 +1645,9 @@
       <c r="D10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
+      <c r="E10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
       <c r="O10" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
@@ -1632,12 +1655,12 @@
       <c r="R10" s="2"/>
       <c r="W10" s="23"/>
       <c r="Y10" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI10"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35">
       <c r="A11" s="1">
         <v>44319</v>
       </c>
@@ -1647,9 +1670,9 @@
       <c r="D11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
+      <c r="E11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
       <c r="O11" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
@@ -1657,21 +1680,21 @@
       <c r="R11" s="2"/>
       <c r="W11" s="23"/>
       <c r="Y11" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI11"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35">
       <c r="A12" s="1">
         <v>44326</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
+      <c r="E12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
       <c r="O12" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
@@ -1679,12 +1702,12 @@
       <c r="R12" s="2"/>
       <c r="W12" s="23"/>
       <c r="Y12" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI12"/>
     </row>
-    <row r="13" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" s="2" customFormat="1">
       <c r="A13" s="3">
         <v>44333</v>
       </c>
@@ -1707,7 +1730,7 @@
       <c r="J13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="34" t="s">
+      <c r="L13" s="32" t="s">
         <v>81</v>
       </c>
       <c r="M13" s="24"/>
@@ -1725,6 +1748,9 @@
       <c r="R13" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="T13" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1732,15 +1758,15 @@
       <c r="X13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y13" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-05-17-swc-gapminder-R</v>
+      <c r="Y13" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-05-17-swc-gapminder-R</v>
       </c>
       <c r="Z13" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" s="2" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>82</v>
@@ -1764,7 +1790,7 @@
       <c r="J14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="34"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
       <c r="O14" s="5" t="str">
@@ -1774,6 +1800,9 @@
       <c r="P14" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="T14" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1781,15 +1810,15 @@
       <c r="X14" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y14" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-05-17</v>
+      <c r="Y14" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-05-17</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35">
       <c r="A15" s="1">
         <v>44340</v>
       </c>
@@ -1799,9 +1828,9 @@
       <c r="D15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
+      <c r="E15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
       <c r="O15" s="10" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
@@ -1809,12 +1838,12 @@
       <c r="R15" s="2"/>
       <c r="W15" s="23"/>
       <c r="Y15" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI15"/>
     </row>
-    <row r="16" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" s="2" customFormat="1">
       <c r="A16" s="3">
         <v>44347</v>
       </c>
@@ -1834,7 +1863,7 @@
       <c r="I16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="34" t="s">
+      <c r="L16" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M16" s="24"/>
@@ -1849,6 +1878,9 @@
       <c r="Q16" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="T16" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1856,15 +1888,15 @@
       <c r="X16" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y16" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-06-02-ds-gpu</v>
+      <c r="Y16" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-06-02-ds-gpu</v>
       </c>
       <c r="Z16" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" s="6" customFormat="1">
       <c r="A17" s="7">
         <v>44354</v>
       </c>
@@ -1890,7 +1922,7 @@
       <c r="K17" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="L17" s="35"/>
+      <c r="L17" s="33"/>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
       <c r="O17" s="6" t="str">
@@ -1903,6 +1935,9 @@
       <c r="Q17" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="T17" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="U17" s="6" t="s">
         <v>40</v>
       </c>
@@ -1910,15 +1945,15 @@
       <c r="X17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Y17" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-06-07-ds-cr</v>
+      <c r="Y17" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-06-07-ds-cr</v>
       </c>
       <c r="Z17" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" s="6" customFormat="1">
       <c r="A18" s="7">
         <v>44361</v>
       </c>
@@ -1941,13 +1976,16 @@
       <c r="J18" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="35"/>
+      <c r="L18" s="33"/>
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
       <c r="O18" s="8" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v>2021-06-14</v>
       </c>
+      <c r="T18" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="U18" s="6" t="s">
         <v>40</v>
       </c>
@@ -1955,15 +1993,15 @@
       <c r="X18" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Y18" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-06-14</v>
+      <c r="Y18" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-06-14</v>
       </c>
       <c r="Z18" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35">
       <c r="A19" s="1">
         <v>44368</v>
       </c>
@@ -1982,12 +2020,12 @@
       </c>
       <c r="W19" s="23"/>
       <c r="Y19" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI19"/>
     </row>
-    <row r="20" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" s="2" customFormat="1">
       <c r="A20" s="3">
         <v>44376</v>
       </c>
@@ -2010,7 +2048,7 @@
       <c r="I20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="32" t="s">
         <v>105</v>
       </c>
       <c r="M20" s="24"/>
@@ -2025,6 +2063,9 @@
       <c r="Q20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="T20" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="U20" s="2" t="s">
         <v>40</v>
       </c>
@@ -2032,15 +2073,15 @@
       <c r="X20" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="Y20" s="34" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-06-28-ds-parallel</v>
+      <c r="Y20" s="32" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-06-28-ds-parallel</v>
       </c>
       <c r="Z20" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" s="6" customFormat="1">
       <c r="A21" s="7">
         <v>44382</v>
       </c>
@@ -2063,7 +2104,7 @@
       <c r="J21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L21" s="35" t="s">
+      <c r="L21" s="33" t="s">
         <v>110</v>
       </c>
       <c r="M21" s="25"/>
@@ -2078,6 +2119,9 @@
       <c r="Q21" s="6" t="s">
         <v>109</v>
       </c>
+      <c r="T21" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="U21" s="6" t="s">
         <v>40</v>
       </c>
@@ -2085,15 +2129,15 @@
       <c r="X21" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Y21" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-07-05-ds-dl-intro</v>
+      <c r="Y21" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-07-05-ds-dl-intro</v>
       </c>
       <c r="Z21" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35">
       <c r="A22" s="1">
         <v>44389</v>
       </c>
@@ -2106,21 +2150,21 @@
       <c r="D22" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
+      <c r="E22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
       <c r="O22" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W22" s="23"/>
       <c r="Y22" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI22"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="A23" s="1">
         <v>44396</v>
       </c>
@@ -2130,21 +2174,21 @@
       <c r="D23" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
+      <c r="E23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
       <c r="O23" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W23" s="23"/>
       <c r="Y23" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI23"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35">
       <c r="A24" s="1">
         <v>44403</v>
       </c>
@@ -2154,21 +2198,21 @@
       <c r="D24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
+      <c r="E24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
       <c r="O24" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W24" s="23"/>
       <c r="Y24" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI24"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="A25" s="1">
         <v>44410</v>
       </c>
@@ -2178,21 +2222,21 @@
       <c r="D25" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
+      <c r="E25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
       <c r="O25" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W25" s="23"/>
       <c r="Y25" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI25"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="A26" s="1">
         <v>44417</v>
       </c>
@@ -2202,21 +2246,21 @@
       <c r="D26" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
+      <c r="E26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
       <c r="O26" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W26" s="23"/>
       <c r="Y26" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI26"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35">
       <c r="A27" s="1">
         <v>44424</v>
       </c>
@@ -2226,21 +2270,21 @@
       <c r="D27" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
+      <c r="E27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
       <c r="O27" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W27" s="23"/>
       <c r="Y27" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI27"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="A28" s="1">
         <v>44431</v>
       </c>
@@ -2250,21 +2294,21 @@
       <c r="D28" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
+      <c r="E28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
       <c r="O28" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W28" s="23"/>
       <c r="Y28" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI28"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="A29" s="1">
         <v>44438</v>
       </c>
@@ -2274,28 +2318,28 @@
       <c r="D29" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
+      <c r="E29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
       <c r="O29" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W29" s="23"/>
       <c r="Y29" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI29"/>
     </row>
-    <row r="30" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" s="6" customFormat="1">
       <c r="A30" s="7">
         <v>44445</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="37" t="s">
         <v>113</v>
       </c>
       <c r="E30" s="25" t="s">
@@ -2316,7 +2360,7 @@
       <c r="J30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L30" s="35" t="s">
+      <c r="L30" s="33" t="s">
         <v>119</v>
       </c>
       <c r="M30" s="25" t="s">
@@ -2340,6 +2384,9 @@
       </c>
       <c r="S30" s="6" t="s">
         <v>39</v>
+      </c>
+      <c r="T30" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="U30" s="6" t="s">
         <v>40</v>
@@ -2348,22 +2395,22 @@
       <c r="X30" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Y30" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-09-06-swc-gapminder-python-nlesc</v>
+      <c r="Y30" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-09-06-swc-gapminder-python-nlesc</v>
       </c>
       <c r="Z30" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" s="6" customFormat="1">
       <c r="A31" s="7">
         <v>44452</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="37" t="s">
         <v>120</v>
       </c>
       <c r="E31" s="25" t="s">
@@ -2384,7 +2431,7 @@
       <c r="K31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L31" s="35"/>
+      <c r="L31" s="33"/>
       <c r="M31" s="25" t="s">
         <v>115</v>
       </c>
@@ -2393,13 +2440,16 @@
       </c>
       <c r="O31" s="8" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
-        <v>2021-09-15-ds-containers</v>
+        <v>2021-09-15-ds-docker</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>48</v>
       </c>
       <c r="Q31" s="6" t="s">
-        <v>49</v>
+        <v>177</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="U31" s="6" t="s">
         <v>40</v>
@@ -2408,20 +2458,20 @@
       <c r="X31" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Y31" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-09-15-ds-containers</v>
+      <c r="Y31" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-09-15-ds-docker</v>
       </c>
       <c r="Z31" s="9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35">
       <c r="A32" s="1">
         <v>44459</v>
       </c>
       <c r="B32"/>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="38" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="23"/>
@@ -2433,17 +2483,17 @@
       </c>
       <c r="W32" s="23"/>
       <c r="Y32" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI32"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35">
       <c r="A33" s="1">
         <v>44466</v>
       </c>
       <c r="B33"/>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="38" t="s">
         <v>25</v>
       </c>
       <c r="E33" s="23"/>
@@ -2455,75 +2505,78 @@
       </c>
       <c r="W33" s="23"/>
       <c r="Y33" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI33"/>
     </row>
-    <row r="34" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+    <row r="34" spans="1:35" s="6" customFormat="1">
+      <c r="A34" s="7">
         <v>44473</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="14" t="s">
+      <c r="E34" s="25"/>
+      <c r="F34" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L34" s="36" t="s">
+      <c r="L34" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="14" t="str">
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="6" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v>2021-10-04-ds-cr</v>
       </c>
-      <c r="P34" s="14" t="s">
+      <c r="P34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q34" s="14" t="s">
+      <c r="Q34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="U34" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="W34" s="22"/>
-      <c r="Y34" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-10-04-ds-cr</v>
-      </c>
-      <c r="Z34" s="14" t="s">
+      <c r="T34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="U34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W34" s="25"/>
+      <c r="Y34" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-10-04-ds-cr</v>
+      </c>
+      <c r="Z34" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="AB34" s="14" t="s">
+      <c r="AB34" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" s="14" customFormat="1">
       <c r="A35" s="13">
         <v>44480</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="39" t="s">
         <v>127</v>
       </c>
       <c r="E35" s="22"/>
@@ -2533,26 +2586,29 @@
       <c r="I35" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="36"/>
+      <c r="L35" s="34"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="15" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v>2021-10-11</v>
       </c>
+      <c r="T35" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="U35" s="14" t="s">
         <v>40</v>
       </c>
       <c r="W35" s="22"/>
-      <c r="Y35" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-10-11</v>
+      <c r="Y35" s="34" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-10-11</v>
       </c>
       <c r="Z35" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" s="14" customFormat="1">
       <c r="A36" s="13">
         <v>44487</v>
       </c>
@@ -2569,7 +2625,7 @@
       <c r="I36" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L36" s="36" t="s">
+      <c r="L36" s="34" t="s">
         <v>134</v>
       </c>
       <c r="M36" s="22"/>
@@ -2590,19 +2646,22 @@
       <c r="S36" s="14" t="s">
         <v>39</v>
       </c>
+      <c r="T36" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="U36" s="14" t="s">
         <v>40</v>
       </c>
       <c r="W36" s="22"/>
-      <c r="Y36" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-10-18-dc-geospatial-python-nlesc</v>
+      <c r="Y36" s="34" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-10-18-dc-geospatial-python-nlesc</v>
       </c>
       <c r="Z36" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35">
       <c r="A37" s="1">
         <v>44494</v>
       </c>
@@ -2612,21 +2671,21 @@
       <c r="D37" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
+      <c r="E37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
       <c r="O37" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W37" s="23"/>
       <c r="Y37" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI37"/>
     </row>
-    <row r="38" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35" s="6" customFormat="1">
       <c r="A38" s="7">
         <v>44501</v>
       </c>
@@ -2649,7 +2708,7 @@
       <c r="J38" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="L38" s="35"/>
+      <c r="L38" s="33"/>
       <c r="M38" s="25"/>
       <c r="N38" s="25"/>
       <c r="O38" s="6" t="str">
@@ -2662,19 +2721,22 @@
       <c r="Q38" s="6" t="s">
         <v>91</v>
       </c>
+      <c r="T38" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="U38" s="6" t="s">
         <v>40</v>
       </c>
       <c r="W38" s="25"/>
-      <c r="Y38" s="35" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-11-01-ds-gpu</v>
+      <c r="Y38" s="33" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-11-01-ds-gpu</v>
       </c>
       <c r="Z38" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" s="14" customFormat="1">
       <c r="A39" s="13">
         <v>44508</v>
       </c>
@@ -2697,7 +2759,7 @@
       <c r="J39" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="L39" s="36"/>
+      <c r="L39" s="34"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="19" t="str">
@@ -2710,40 +2772,43 @@
       <c r="Q39" s="14" t="s">
         <v>63</v>
       </c>
+      <c r="T39" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="U39" s="14" t="s">
         <v>40</v>
       </c>
       <c r="W39" s="22"/>
-      <c r="Y39" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-11-08-ds-parallel</v>
+      <c r="Y39" s="34" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-11-08-ds-parallel</v>
       </c>
       <c r="Z39" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" s="10" customFormat="1">
       <c r="A40" s="11">
         <v>44515</v>
       </c>
       <c r="D40" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
+      <c r="E40" s="28"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
       <c r="O40" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
-      <c r="W40" s="30"/>
-      <c r="Y40" s="37" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W40" s="28"/>
+      <c r="Y40" s="35" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:35" s="14" customFormat="1">
       <c r="A41" s="13">
         <v>44522</v>
       </c>
@@ -2760,7 +2825,7 @@
       <c r="I41" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="L41" s="36" t="s">
+      <c r="L41" s="34" t="s">
         <v>143</v>
       </c>
       <c r="M41" s="22"/>
@@ -2775,19 +2840,22 @@
       <c r="Q41" s="14" t="s">
         <v>109</v>
       </c>
+      <c r="T41" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="U41" s="14" t="s">
         <v>40</v>
       </c>
       <c r="W41" s="22"/>
-      <c r="Y41" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-11-20-ds-dl-intro</v>
+      <c r="Y41" s="34" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-11-20-ds-dl-intro</v>
       </c>
       <c r="Z41" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35">
       <c r="A42" s="1">
         <v>44529</v>
       </c>
@@ -2797,21 +2865,21 @@
       <c r="D42" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="E42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
       <c r="O42" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v/>
       </c>
       <c r="W42" s="23"/>
       <c r="Y42" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI42"/>
     </row>
-    <row r="43" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:35" s="14" customFormat="1">
       <c r="A43" s="13">
         <v>44536</v>
       </c>
@@ -2828,7 +2896,7 @@
       <c r="G43" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="L43" s="36"/>
+      <c r="L43" s="34"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="15" t="str">
@@ -2847,19 +2915,22 @@
       <c r="S43" s="14" t="s">
         <v>39</v>
       </c>
+      <c r="T43" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="U43" s="14" t="s">
         <v>40</v>
       </c>
       <c r="W43" s="22"/>
-      <c r="Y43" s="36" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-12-06-dc-socsci-python-nlesc</v>
+      <c r="Y43" s="34" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-12-06-dc-socsci-python-nlesc</v>
       </c>
       <c r="Z43" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:35">
       <c r="A44" s="1">
         <v>44543</v>
       </c>
@@ -2877,80 +2948,80 @@
       </c>
       <c r="W44" s="23"/>
       <c r="Y44" s="18" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
         <v/>
       </c>
       <c r="AI44"/>
     </row>
-    <row r="45" spans="1:35" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="31">
+    <row r="45" spans="1:35" s="30" customFormat="1">
+      <c r="A45" s="29">
         <v>44550</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="E45" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G45" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="32" t="s">
+      <c r="H45" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="I45" s="32" t="s">
+      <c r="I45" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="J45" s="32" t="s">
+      <c r="J45" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="L45" s="38"/>
-      <c r="M45" s="33" t="s">
+      <c r="L45" s="36"/>
+      <c r="M45" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="N45" s="33" t="s">
+      <c r="N45" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="O45" s="32" t="str">
+      <c r="O45" s="30" t="str">
         <f>_xlfn.TEXTJOIN("-", TRUE, Table1[[#This Row],[startdate]], Table1[[#This Row],[curriculum]], Table1[[#This Row],[flavor]], Table1[[#This Row],[host]])</f>
         <v>2021-12-24-dc-socsci-R-nlesc</v>
       </c>
-      <c r="P45" s="32" t="s">
+      <c r="P45" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="Q45" s="32" t="s">
+      <c r="Q45" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="R45" s="32" t="s">
+      <c r="R45" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="S45" s="32" t="s">
+      <c r="S45" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="T45" s="32" t="s">
+      <c r="T45" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="U45" s="32" t="s">
+      <c r="U45" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="V45" s="32" t="s">
+      <c r="V45" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="W45" s="33" t="s">
+      <c r="W45" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="Y45" s="38" t="str">
-        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/escience-academy", Table1[[#This Row],[slug]]),"")</f>
-        <v>https://github.com/escience-academy/2021-12-24-dc-socsci-R-nlesc</v>
+      <c r="Y45" s="36" t="str">
+        <f>IF(Table1[[#This Row],[slug]]&lt;&gt;"",_xlfn.TEXTJOIN("/", TRUE, "https://github.com/esciencecenter-digital-skills", Table1[[#This Row],[slug]]),"")</f>
+        <v>https://github.com/esciencecenter-digital-skills/2021-12-24-dc-socsci-R-nlesc</v>
       </c>
     </row>
   </sheetData>
@@ -3034,19 +3105,19 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" customWidth="1"/>
-    <col min="20" max="20" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -3102,7 +3173,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3153,7 +3224,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -3203,7 +3274,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3229,9 +3300,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>148</v>
@@ -3255,7 +3326,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -3281,7 +3352,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="R7" t="s">
         <v>169</v>
       </c>
@@ -3301,7 +3372,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="R8" t="s">
         <v>68</v>
       </c>
@@ -3321,7 +3392,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="R9" t="s">
         <v>56</v>
       </c>
@@ -3341,7 +3412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="R10" t="s">
         <v>170</v>
       </c>
@@ -3361,7 +3432,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="R11" t="s">
         <v>35</v>
       </c>
@@ -3381,7 +3452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="R12" t="s">
         <v>34</v>
       </c>
@@ -3401,7 +3472,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="R13" t="s">
         <v>171</v>
       </c>
@@ -3421,7 +3492,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="R14" t="s">
         <v>118</v>
       </c>
@@ -3441,7 +3512,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="R15" t="s">
         <v>33</v>
       </c>
@@ -3461,7 +3532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="R16" t="s">
         <v>172</v>
       </c>
@@ -3481,7 +3552,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="R17" t="s">
         <v>46</v>
       </c>
@@ -3501,7 +3572,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="R18" t="s">
         <v>62</v>
       </c>
@@ -3521,7 +3592,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -3544,7 +3615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3567,7 +3638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -3590,7 +3661,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3613,7 +3684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -3636,7 +3707,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -3659,7 +3730,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23">
       <c r="R25" t="s">
         <v>85</v>
       </c>
@@ -3679,7 +3750,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23">
       <c r="R26" t="s">
         <v>54</v>
       </c>
@@ -3699,7 +3770,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23">
       <c r="R27" t="s">
         <v>97</v>
       </c>
@@ -3719,7 +3790,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23">
       <c r="R28" t="s">
         <v>101</v>
       </c>
@@ -3751,21 +3822,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008C9242AECD975D4DA7B237C2E1E764BE" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c17cf1ac27542d444d37c94d4a806c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="375943d0-1737-420d-abae-750e225a1f6c" xmlns:ns3="dbccc4ca-e175-4642-95d3-c6632d06f78c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a86557ffa725881dffa61df7e15aa77c" ns2:_="" ns3:_="">
     <xsd:import namespace="375943d0-1737-420d-abae-750e225a1f6c"/>
@@ -3976,32 +4032,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C0E574-FBDB-44E9-A84B-01ACC8D8F634}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="375943d0-1737-420d-abae-750e225a1f6c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dbccc4ca-e175-4642-95d3-c6632d06f78c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDBB668-EFC0-4007-8FDF-6AC14434B285}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{163C5686-18A8-4F18-93FF-D790DCEED680}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4018,4 +4064,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EDBB668-EFC0-4007-8FDF-6AC14434B285}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C0E574-FBDB-44E9-A84B-01ACC8D8F634}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="375943d0-1737-420d-abae-750e225a1f6c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dbccc4ca-e175-4642-95d3-c6632d06f78c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>